<commit_message>
Added a lot TODOs
</commit_message>
<xml_diff>
--- a/generated-statistics-file.xlsx
+++ b/generated-statistics-file.xlsx
@@ -1060,6 +1060,9 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>410.0</v>
+      </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -1110,6 +1113,9 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>396.0</v>
+      </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -1160,6 +1166,9 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="n">
+        <v>413.0</v>
+      </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -1210,6 +1219,9 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="n">
+        <v>392.0</v>
+      </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1260,6 +1272,9 @@
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="n">
+        <v>390.0</v>
+      </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1310,6 +1325,9 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="n">
+        <v>419.0</v>
+      </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -1360,6 +1378,9 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="n">
+        <v>397.0</v>
+      </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -1410,6 +1431,9 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="n">
+        <v>394.0</v>
+      </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -1460,6 +1484,9 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="n">
+        <v>446.0</v>
+      </c>
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -1510,6 +1537,9 @@
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="n">
+        <v>432.0</v>
+      </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
@@ -1560,6 +1590,9 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="n">
+        <v>391.0</v>
+      </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -1610,6 +1643,9 @@
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="n">
+        <v>404.0</v>
+      </c>
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -1660,6 +1696,9 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="n">
+        <v>407.0</v>
+      </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
@@ -1710,6 +1749,9 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="n">
+        <v>393.0</v>
+      </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -1760,6 +1802,9 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="n">
+        <v>405.0</v>
+      </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
@@ -1810,6 +1855,9 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="n">
+        <v>410.0</v>
+      </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
@@ -1860,6 +1908,9 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="n">
+        <v>396.0</v>
+      </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -1910,6 +1961,9 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="n">
+        <v>413.0</v>
+      </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
@@ -1960,6 +2014,9 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="n">
+        <v>392.0</v>
+      </c>
       <c r="B20" t="s">
         <v>34</v>
       </c>
@@ -2010,6 +2067,9 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="n">
+        <v>390.0</v>
+      </c>
       <c r="B21" t="s">
         <v>35</v>
       </c>
@@ -2060,6 +2120,9 @@
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="n">
+        <v>446.0</v>
+      </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
@@ -2110,6 +2173,9 @@
       </c>
     </row>
     <row r="23">
+      <c r="A23" t="n">
+        <v>419.0</v>
+      </c>
       <c r="B23" t="s">
         <v>37</v>
       </c>
@@ -2160,6 +2226,9 @@
       </c>
     </row>
     <row r="24">
+      <c r="A24" t="n">
+        <v>432.0</v>
+      </c>
       <c r="B24" t="s">
         <v>38</v>
       </c>
@@ -2210,6 +2279,9 @@
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="n">
+        <v>397.0</v>
+      </c>
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -2260,6 +2332,9 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="n">
+        <v>391.0</v>
+      </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
@@ -2310,6 +2385,9 @@
       </c>
     </row>
     <row r="27">
+      <c r="A27" t="n">
+        <v>394.0</v>
+      </c>
       <c r="B27" t="s">
         <v>41</v>
       </c>
@@ -2360,6 +2438,9 @@
       </c>
     </row>
     <row r="28">
+      <c r="A28" t="n">
+        <v>404.0</v>
+      </c>
       <c r="B28" t="s">
         <v>42</v>
       </c>
@@ -2410,6 +2491,9 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="n">
+        <v>407.0</v>
+      </c>
       <c r="B29" t="s">
         <v>43</v>
       </c>
@@ -2460,6 +2544,9 @@
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="n">
+        <v>393.0</v>
+      </c>
       <c r="B30" t="s">
         <v>44</v>
       </c>
@@ -2510,6 +2597,9 @@
       </c>
     </row>
     <row r="31">
+      <c r="A31" t="n">
+        <v>405.0</v>
+      </c>
       <c r="B31" t="s">
         <v>45</v>
       </c>

</xml_diff>